<commit_message>
Response to Andrew's comments regarding the new "eCitation/Ticket"
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="6400" yWindow="1460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -1310,34 +1310,159 @@
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationCountyName</t>
   </si>
   <si>
-    <t>How do we know this is a ticket?</t>
-  </si>
-  <si>
-    <t>Couldn’t this be better modeled as a role or an association?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instead of "ticket" the proper term is probably "citation".  Also, can you please check the definition of this element in schema, doesn’t seem right. </t>
-  </si>
-  <si>
-    <t>Wouldn't it be better to derive this from an association? That is an association between the ticket at the organization it was issued to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">can we insert another node level in here for "TicketNotarization" or "CitationNotarization" and a property of that would be the date.  There' a chance that there will be other notarization detail </t>
-  </si>
-  <si>
-    <t>Presumably there is an association between the ticket at he organization to make it clear that the organization received the ticket?</t>
-  </si>
-  <si>
-    <t>If there are multiple people in the report, how do we know which one received the ticket?</t>
-  </si>
-  <si>
-    <t>We should also include the Xpath for residence association to indicate that a location needs to be association to a person</t>
-  </si>
-  <si>
-    <t>Wouldn’t this be better modeled as a property of a driver license, not a person?</t>
-  </si>
-  <si>
-    <t>Let's spell this out, not FAW acronym unless that is a commonly used acronym of which I am not aware</t>
+    <t>It isn't clear to me how we know this person is associated to the county above for the purpose of notary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How do we know this is a ticket?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I'm not sure about your question, Vermont calls this a "Ticket Number"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Couldn’t this be better modeled as a role or an association?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I can do that.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Instead of "ticket" the proper term is probably "citation".  Also, can you please check the definition of this element in schema, doesn’t seem right. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I'll change all occurences of "Ticket" to "Citation" and check definitions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wouldn't it be better to derive this from an association? That is an association between the ticket at the organization it was issued to
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I can do that.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">can we insert another node level in here for "TicketNotarization" or "CitationNotarization" and a property of that would be the date.  There' a chance that there will be other notarization detail 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I can do that.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Presumably there is an association between the ticket at he organization to make it clear that the organization received the ticket?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yes there is.  I'll include the Association in the spreadsheet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If there are multiple people in the report, how do we know which one received the ticket?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ticket (Citation) Incident Association
+Person In cident Association
+I'll include Associations in tha mapping</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We should also include the Xpath for residence association to indicate that a location needs to be association to a person
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I'll include the Associations in the mapping.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wouldn’t this be better modeled as a property of a driver license, not a person?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Agreed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Let's spell this out, not FAW acronym unless that is a commonly used acronym of which I am not aware
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OK</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1360,17 +1485,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/nc:ActivityIdentification/nc:IdentificationID</t>
+      <t xml:space="preserve">/nc:ActivityIdentification/nc:IdentificationID
+</t>
     </r>
-  </si>
-  <si>
-    <t>there isn't a concept for this in NIEM or N-Dex?</t>
-  </si>
-  <si>
-    <t>We should indicate the Association Xpath in here</t>
-  </si>
-  <si>
-    <t>It isn't clear to me how we know this person is associated to the county above for the purpose of notary</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">there isn't a concept for this in NIEM or N-Dex?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NIEM only has "ArrestBloodAlcoholContentNumberText"
+ECF has "PersonBloodAlcoholNumber"… I can use this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We should indicate the Association Xpath in here
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I'll add Associations to the spreadsheet</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2401,7 +2558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2411,7 +2568,8 @@
     <col min="3" max="4" width="29.6640625" style="13" customWidth="1"/>
     <col min="5" max="5" width="105.83203125" style="13" customWidth="1"/>
     <col min="6" max="6" width="57.33203125" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="13"/>
+    <col min="7" max="7" width="48.1640625" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="27" customFormat="1" ht="47" customHeight="1">
@@ -2471,7 +2629,7 @@
         <v>319</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="16" customFormat="1" ht="42">
@@ -2491,10 +2649,10 @@
         <v>384</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="16" customFormat="1" ht="56">
       <c r="A6" s="20" t="s">
         <v>230</v>
       </c>
@@ -2511,7 +2669,7 @@
         <v>363</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="16" customFormat="1" ht="42">
@@ -2566,7 +2724,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="16" customFormat="1" ht="42">
+    <row r="10" spans="1:6" s="16" customFormat="1" ht="56">
       <c r="A10" s="20" t="s">
         <v>240</v>
       </c>
@@ -2583,10 +2741,10 @@
         <v>385</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="42">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="70">
       <c r="A11" s="21" t="s">
         <v>267</v>
       </c>
@@ -2603,7 +2761,7 @@
         <v>367</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2616,7 +2774,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:6" ht="42">
+    <row r="13" spans="1:6" ht="56">
       <c r="A13" s="13" t="s">
         <v>133</v>
       </c>
@@ -2630,7 +2788,7 @@
         <v>339</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2643,7 +2801,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:6" ht="42">
+    <row r="15" spans="1:6" ht="84">
       <c r="A15" s="13" t="s">
         <v>202</v>
       </c>
@@ -2660,7 +2818,7 @@
         <v>322</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="42">
@@ -2697,7 +2855,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="42">
+    <row r="18" spans="1:6" ht="56">
       <c r="A18" s="13" t="s">
         <v>192</v>
       </c>
@@ -2714,7 +2872,7 @@
         <v>344</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="42">
@@ -2785,7 +2943,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="42">
+    <row r="23" spans="1:6" ht="56">
       <c r="A23" s="21" t="s">
         <v>234</v>
       </c>
@@ -2802,7 +2960,7 @@
         <v>380</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="42">
@@ -2822,7 +2980,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="42">
+    <row r="25" spans="1:6" ht="56">
       <c r="A25" s="21" t="s">
         <v>233</v>
       </c>
@@ -2839,7 +2997,7 @@
         <v>379</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="16" customFormat="1" ht="42">
@@ -3188,7 +3346,7 @@
       <c r="E47" s="19"/>
       <c r="F47" s="19"/>
     </row>
-    <row r="48" spans="1:6" s="16" customFormat="1" ht="70">
+    <row r="48" spans="1:6" s="16" customFormat="1" ht="98">
       <c r="A48" s="13" t="s">
         <v>249</v>
       </c>
@@ -3205,7 +3363,7 @@
         <v>274</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="16" customFormat="1" ht="22.5" customHeight="1">
@@ -3291,7 +3449,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="16" customFormat="1" ht="42">
+    <row r="54" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A54" s="20" t="s">
         <v>255</v>
       </c>
@@ -3308,7 +3466,7 @@
         <v>371</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="16" customFormat="1" ht="42">
@@ -3760,7 +3918,7 @@
         <v>321</v>
       </c>
       <c r="F82" s="16" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="42">
@@ -3896,7 +4054,7 @@
         <v>323</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28">

</xml_diff>

<commit_message>
Updates to Citation XML instance and XPATH mapping.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="1460" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="680" yWindow="240" windowWidth="28800" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="409">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -442,9 +442,6 @@
     <t>Lic. State</t>
   </si>
   <si>
-    <t>Ticket Number</t>
-  </si>
-  <si>
     <t>Driver License No.</t>
   </si>
   <si>
@@ -472,9 +469,6 @@
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Corp/Org</t>
-  </si>
-  <si>
     <t>POB</t>
   </si>
   <si>
@@ -706,21 +700,9 @@
     <t>PARENT/GAURDIAN</t>
   </si>
   <si>
-    <t>OFFICIAL</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
-    <t>Ticket Served Date</t>
-  </si>
-  <si>
-    <t>Ticket Served Indicator</t>
-  </si>
-  <si>
-    <t>Ticket Mailed Indicator</t>
-  </si>
-  <si>
     <t>Fish &amp; Wildlife License Number</t>
   </si>
   <si>
@@ -742,12 +724,6 @@
     <t>Middle Name or Initial</t>
   </si>
   <si>
-    <t>Ticket Receipient Organization Indicator</t>
-  </si>
-  <si>
-    <t>Ticket Delivered Receipient</t>
-  </si>
-  <si>
     <t>Vehicle Plate Number</t>
   </si>
   <si>
@@ -823,9 +799,6 @@
     <t>Official Number</t>
   </si>
   <si>
-    <t>Ticket Notarized Date</t>
-  </si>
-  <si>
     <t>Notary County</t>
   </si>
   <si>
@@ -841,15 +814,6 @@
     <t>Offense Fine Maximum Amount</t>
   </si>
   <si>
-    <t>Vermont eTicket Element</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
     <t>Sample Data</t>
   </si>
   <si>
@@ -973,114 +937,24 @@
     <t>Commerical Vehicle Indicator</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
     <t>This element appears to be a duplicate of the Officer Agency ORI.  We need to know what this element should be.</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/nc:DocumentIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonName/nc:PersonFullName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Hair Color Code</t>
   </si>
   <si>
     <t>Eye Color Code</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonEyeColorCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonHairColorCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonHeightMeasure/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
     <t>Place Of Birth</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonSexCode</t>
-  </si>
-  <si>
     <t>Height Unit</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonWeightMeasure/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/nc:PersonWeightMeasure/nc:WeightUnitCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization/nc:OrganizationName</t>
-  </si>
-  <si>
     <t>ACME</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:VehicleColorPrimaryCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:ItemModelYearDate</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:VehicleStyleCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationJurisdictionFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:VehicleMakeCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Organization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Vehicle/nc:VehicleCMVIndicator</t>
-  </si>
-  <si>
     <t>CFR Statute Code</t>
   </si>
   <si>
@@ -1111,75 +985,9 @@
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Charge/inc-ext:RelatedCriminalChargeIndicator</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketServedDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:WaiverAmount</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketServedIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketMailedIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketNotarizedDate</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Vehicle/inc-ext:VehicleHazardousMaterialIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/j:DrivingIncidentRecordedSpeedRate/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/j:DrivingIncidentLegalSpeedRate/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:BloodAlcoholContentNumberText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:DrivingAccidentIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:DrivingAccidentFatalityIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:SeatBeltViolationIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:CityReliefActIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:CityReliefActJuvenileIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:CityReliefActOtherIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/inc-ext:CityReliefActOtherText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Person/inc-ext:PersonFAWLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Person/inc-ext:PersonDriverLicenseCDLIndicator</t>
-  </si>
-  <si>
     <t>VIN</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/nc:VehicleIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Offense/inc-ext:OffenseViolatedStatute/j:StatuteCodeIdentification</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketDeliveredRecipientText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Ticket/inc-ext:TicketRecipientOrganizationIndicator</t>
-  </si>
-  <si>
     <t>Speed Unit of Measure</t>
   </si>
   <si>
@@ -1219,27 +1027,9 @@
     <t>Complaint number assigned by the court.</t>
   </si>
   <si>
-    <t>The entity that received the ticket.</t>
-  </si>
-  <si>
-    <t>The date the ticket was served to the subject.</t>
-  </si>
-  <si>
     <t>The amount paid for an admitted or no contest plea.</t>
   </si>
   <si>
-    <t>Indicates that the ticket/citation was handed to the subject.</t>
-  </si>
-  <si>
-    <t>Indicates that theticket/citation was mailed to the subject.</t>
-  </si>
-  <si>
-    <t>Indicates that the ticketed entity is a corporation or organization.</t>
-  </si>
-  <si>
-    <t>The date that the ticket was notarized.</t>
-  </si>
-  <si>
     <t>The name of the organization that is the subject.</t>
   </si>
   <si>
@@ -1276,148 +1066,13 @@
     <t>Indicates that there is a related criminal charge</t>
   </si>
   <si>
-    <t>eTicket Element
-(Elements in RED are OJB extensions to the base Incident)</t>
-  </si>
-  <si>
-    <t>Should we use a code table for this element?</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
     <t>Actual speed unit of measure</t>
   </si>
   <si>
     <t>Posteds peed unit of measure</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationDescriptionText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationHighway/nc:HighwayID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationHighway/nc:HighwayPositionText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationCountyName</t>
-  </si>
-  <si>
     <t>It isn't clear to me how we know this person is associated to the county above for the purpose of notary</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">How do we know this is a ticket?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I'm not sure about your question, Vermont calls this a "Ticket Number"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Couldn’t this be better modeled as a role or an association?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I can do that.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Instead of "ticket" the proper term is probably "citation".  Also, can you please check the definition of this element in schema, doesn’t seem right. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I'll change all occurences of "Ticket" to "Citation" and check definitions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Wouldn't it be better to derive this from an association? That is an association between the ticket at the organization it was issued to
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I can do that.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">can we insert another node level in here for "TicketNotarization" or "CitationNotarization" and a property of that would be the date.  There' a chance that there will be other notarization detail 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I can do that.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Presumably there is an association between the ticket at he organization to make it clear that the organization received the ticket?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Yes there is.  I'll include the Association in the spreadsheet</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If there are multiple people in the report, how do we know which one received the ticket?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ticket (Citation) Incident Association
-Person In cident Association
-I'll include Associations in tha mapping</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1529,6 +1184,182 @@
       <t>I'll add Associations to the spreadsheet</t>
     </r>
   </si>
+  <si>
+    <t>CITATION NOTARIZATION</t>
+  </si>
+  <si>
+    <t>eCitation Element
+(Elements in RED are OJB extensions to the base Incident)</t>
+  </si>
+  <si>
+    <t>Vermont eCitation Element</t>
+  </si>
+  <si>
+    <t>Citation Number</t>
+  </si>
+  <si>
+    <t>Citation Delivered Receipient</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/inc-ext:CitationDeliveredRecipientText</t>
+  </si>
+  <si>
+    <t>Citation Served Date</t>
+  </si>
+  <si>
+    <t>Citation Served Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/inc-ext:CitationServedIndicator</t>
+  </si>
+  <si>
+    <t>Citation Mailed Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/inc-ext:CitationMailedIndicator</t>
+  </si>
+  <si>
+    <t>Citation Notarized Date</t>
+  </si>
+  <si>
+    <t>can we insert another node level in here for "CitationNotarization" or "CitationNotarization" and a property of that would be the date.  There' a chance that there will be other notarization detail 
+I can do that.</t>
+  </si>
+  <si>
+    <t>How do we know this is a citation?
+I'm not sure about your question, Vermont calls this a "Citation Number"</t>
+  </si>
+  <si>
+    <t>The entity that received the citation.</t>
+  </si>
+  <si>
+    <t>The date the citation was served to the subject.</t>
+  </si>
+  <si>
+    <t>Instead of "citation" the proper term is probably "citation".  Also, can you please check the definition of this element in schema, doesn’t seem right. 
+I'll change all occurences of "Citation" to "Citation" and check definitions</t>
+  </si>
+  <si>
+    <t>Indicates that the citation/citation was handed to the subject.</t>
+  </si>
+  <si>
+    <t>Indicates that thecitation/citation was mailed to the subject.</t>
+  </si>
+  <si>
+    <t>Presumably there is an association between the citation at he organization to make it clear that the organization received the citation?
+Yes there is.  I'll include the Association in the spreadsheet</t>
+  </si>
+  <si>
+    <t>If there are multiple people in the report, how do we know which one received the citation?
+Citation (Citation) Incident Association
+Person In cident Association
+I'll include Associations in tha mapping</t>
+  </si>
+  <si>
+    <t>The date that the citation was notarized.</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/inc-ext:CitationWaiverAmount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Let's discuss
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I can do that.</t>
+    </r>
+  </si>
+  <si>
+    <t>LICENSE</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationJurisdictionFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Offense/inc-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document[@s:id= /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/lexslib:SameAsDigestReference/@lexslib:ref]/nc:DocumentIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:WeightUnitCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ActivityInvolvedOrganizationAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>ANDREW</t>
+  </si>
 </sst>
 </file>
 
@@ -1537,7 +1368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1678,6 +1509,25 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1786,7 +1636,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="190">
+  <cellStyleXfs count="380">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1977,8 +1827,198 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2064,8 +2104,29 @@
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="190">
+  <cellStyles count="380">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2169,6 +2230,101 @@
     <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2251,6 +2407,101 @@
     <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2556,40 +2807,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35" style="13" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="13" customWidth="1"/>
-    <col min="3" max="4" width="29.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="105.83203125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="34" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.83203125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="57.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="13" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" ht="47" customHeight="1">
+    <row r="1" spans="1:6" s="27" customFormat="1" ht="42">
       <c r="A1" s="11" t="s">
-        <v>418</v>
+        <v>358</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>273</v>
+        <v>359</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>137</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2597,912 +2849,866 @@
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6" ht="42">
+    <row r="4" spans="1:6" ht="70">
       <c r="A4" s="13" t="s">
-        <v>140</v>
+        <v>360</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>398</v>
+        <v>334</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>140</v>
+        <v>360</v>
       </c>
       <c r="D4" s="13">
         <v>82734800</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>319</v>
+      <c r="E4" s="29" t="s">
+        <v>392</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>430</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A5" s="20" t="s">
-        <v>241</v>
+        <v>361</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>384</v>
+        <v>291</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>362</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>431</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="16" customFormat="1" ht="56">
       <c r="A6" s="20" t="s">
-        <v>230</v>
+        <v>363</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>400</v>
+        <v>372</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D6" s="22">
         <v>42304</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>363</v>
+      <c r="E6" s="31" t="s">
+        <v>379</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>432</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A7" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>401</v>
+        <v>335</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D7" s="23">
         <v>105</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>364</v>
+      <c r="E7" s="31" t="s">
+        <v>379</v>
       </c>
       <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A8" s="20" t="s">
-        <v>231</v>
+        <v>364</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>402</v>
+        <v>374</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D8" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="31" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A9" s="20" t="s">
-        <v>232</v>
+        <v>366</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>403</v>
+        <v>375</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D9" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="16" customFormat="1" ht="56">
-      <c r="A10" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>404</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>385</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>433</v>
-      </c>
+      <c r="E9" s="31" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="70">
-      <c r="A11" s="21" t="s">
-        <v>267</v>
+      <c r="A11" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>405</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="24">
-        <v>42305</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>367</v>
+        <v>336</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>407</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>434</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:6" ht="56">
+    <row r="13" spans="1:6" ht="84">
       <c r="A13" s="13" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>406</v>
+        <v>200</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>339</v>
+        <v>267</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>393</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:6" ht="84">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="70">
+      <c r="A14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="70">
       <c r="A15" s="13" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="42">
+        <v>269</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="56">
       <c r="A16" s="13" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="42">
+        <v>270</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="13" t="s">
-        <v>239</v>
+        <v>134</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>239</v>
+        <v>134</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="56">
+        <v>271</v>
+      </c>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="13" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="42">
-      <c r="A19" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="42">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="16" customFormat="1">
+      <c r="A19" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:6" ht="84">
       <c r="A20" s="13" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A21" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="42">
+        <v>140</v>
+      </c>
+      <c r="D20" s="13">
+        <v>41444812</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="84">
+      <c r="A21" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="56">
       <c r="A22" s="13" t="s">
-        <v>49</v>
+        <v>227</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>141</v>
       </c>
       <c r="D22" s="13">
-        <v>41444812</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="56">
-      <c r="A23" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="42">
-      <c r="A24" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="56">
-      <c r="A25" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="13">
         <v>12345678</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="E22" s="35"/>
+      <c r="F22" s="13" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="16" customFormat="1">
+      <c r="A23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="16">
+        <v>8023631111</v>
+      </c>
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="1:6" s="16" customFormat="1">
+      <c r="A24" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="16">
+        <v>8023631112</v>
+      </c>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="1:6" s="16" customFormat="1" ht="70">
+      <c r="A25" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="22">
+        <v>24014</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A26" s="16" t="s">
-        <v>147</v>
+        <v>201</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>409</v>
+        <v>201</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="16">
-        <v>8023631111</v>
-      </c>
-      <c r="E26" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="16" customFormat="1">
+      <c r="A27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A27" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>410</v>
-      </c>
       <c r="C27" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="16">
-        <v>8023631112</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>149</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A28" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" s="22">
-        <v>24014</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>150</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A29" s="16" t="s">
-        <v>203</v>
+        <v>309</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>324</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A30" s="16" t="s">
-        <v>332</v>
+        <v>151</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>411</v>
+        <v>151</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="D30" s="16">
+        <v>135</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A31" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="16" customFormat="1" ht="70">
+      <c r="A32" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A32" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>388</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="D32" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="16" customFormat="1" ht="70">
       <c r="A33" s="16" t="s">
-        <v>153</v>
+        <v>307</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>153</v>
+        <v>307</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A35" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="16" customFormat="1" ht="112">
+      <c r="A36" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="16" customFormat="1" ht="112">
+      <c r="A37" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E33" s="16" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A34" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="D37" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A38" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="16">
+        <v>2015</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A39" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A40" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="E40" s="31" t="s">
         <v>389</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="16" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A35" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A36" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-    </row>
-    <row r="38" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A38" s="16" t="s">
+    </row>
+    <row r="41" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A41" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A42" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="16" customFormat="1" ht="28">
+      <c r="A43" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="31"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="19"/>
+    </row>
+    <row r="45" spans="1:6" s="16" customFormat="1" ht="98">
+      <c r="A45" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="E45" s="20"/>
+      <c r="F45" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="16" customFormat="1">
+      <c r="A46" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="E46" s="31"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" s="16" customFormat="1" ht="28">
+      <c r="A47" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="16" customFormat="1" ht="28">
+      <c r="A48" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="1:6" s="16" customFormat="1" ht="28">
+      <c r="A49" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A39" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="E39" s="16" t="s">
+      <c r="C49" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="1:6" s="16" customFormat="1">
+      <c r="A50" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="E50" s="31"/>
+    </row>
+    <row r="51" spans="1:6" s="16" customFormat="1" ht="70">
+      <c r="A51" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="E51" s="31"/>
+      <c r="F51" s="16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="16" customFormat="1">
+      <c r="A52" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="16">
+        <v>30</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="16" customFormat="1">
+      <c r="A53" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="B53" s="16" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A40" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>390</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A41" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>391</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D41" s="16">
-        <v>2015</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A42" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>392</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A43" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A44" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A45" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>395</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A46" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D46" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-    </row>
-    <row r="48" spans="1:6" s="16" customFormat="1" ht="98">
-      <c r="A48" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="16" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A49" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="F49" s="22"/>
-    </row>
-    <row r="50" spans="1:6" s="16" customFormat="1" ht="28">
-      <c r="A50" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>412</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A51" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>413</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A52" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="B52" s="16" t="s">
+      <c r="D53" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="E53" s="31"/>
+    </row>
+    <row r="54" spans="1:6" s="16" customFormat="1">
+      <c r="A54" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>206</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A53" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>397</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="16" customFormat="1" ht="70">
-      <c r="A54" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>414</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>165</v>
       </c>
       <c r="D54" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>40</v>
+      </c>
+      <c r="E54" s="31"/>
+    </row>
+    <row r="55" spans="1:6" s="16" customFormat="1">
       <c r="A55" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="E55" s="31"/>
+    </row>
+    <row r="56" spans="1:6" s="16" customFormat="1">
+      <c r="A56" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" s="16">
-        <v>30</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A56" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="D56" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="31"/>
+    </row>
+    <row r="57" spans="1:6" s="16" customFormat="1">
       <c r="A57" s="20" t="s">
-        <v>167</v>
+        <v>249</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>208</v>
@@ -3510,190 +3716,178 @@
       <c r="C57" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="D57" s="16">
-        <v>40</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="D57" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="31"/>
+    </row>
+    <row r="58" spans="1:6" s="16" customFormat="1">
       <c r="A58" s="20" t="s">
-        <v>386</v>
+        <v>250</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>422</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A59" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="31"/>
+    </row>
+    <row r="59" spans="1:6" ht="28">
+      <c r="A59" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="28">
+      <c r="A60" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="D59" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A60" s="20" t="s">
+      <c r="B60" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D60" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28">
+      <c r="A61" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="B60" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A61" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D61" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="A64" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="E64" s="31" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="A65" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D61" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="42">
-      <c r="A62" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="D62" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="42">
-      <c r="A63" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="D63" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="42">
-      <c r="A64" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="36" customHeight="1">
-      <c r="A65" s="21" t="s">
+      <c r="C65" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="A66" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="B65" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
+      <c r="B66" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="67" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A67" s="16" t="s">
-        <v>354</v>
+      <c r="A67" s="20" t="s">
+        <v>252</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>416</v>
+        <v>213</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>355</v>
+        <v>290</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A68" s="20" t="s">
-        <v>259</v>
+        <v>319</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>213</v>
+        <v>347</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>383</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D68" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="F68" s="20"/>
     </row>
     <row r="69" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A69" s="26" t="s">
-        <v>353</v>
+      <c r="A69" s="20" t="s">
+        <v>253</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>214</v>
@@ -3701,19 +3895,16 @@
       <c r="C69" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="D69" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>356</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>419</v>
+      <c r="D69" s="16">
+        <v>2</v>
+      </c>
+      <c r="E69" s="31" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A70" s="20" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>215</v>
@@ -3721,354 +3912,324 @@
       <c r="C70" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D70" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="E70" s="16" t="s">
-        <v>357</v>
-      </c>
+      <c r="D70" s="23">
+        <v>47</v>
+      </c>
+      <c r="E70" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="F70" s="23"/>
     </row>
     <row r="71" spans="1:6" s="16" customFormat="1" ht="42">
       <c r="A71" s="20" t="s">
-        <v>361</v>
+        <v>263</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>417</v>
+        <v>216</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D71" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="F71" s="20"/>
-    </row>
-    <row r="72" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A72" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="C72" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D72" s="16">
-        <v>2</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A73" s="20" t="s">
-        <v>271</v>
+      <c r="D71" s="23">
+        <v>1197</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="F71" s="23"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="19"/>
+    </row>
+    <row r="73" spans="1:6" s="16" customFormat="1" ht="70">
+      <c r="A73" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>217</v>
+        <v>184</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D73" s="23">
-        <v>47</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="F73" s="23"/>
-    </row>
-    <row r="74" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A74" s="20" t="s">
-        <v>272</v>
+        <v>184</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="16" customFormat="1">
+      <c r="A74" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="D74" s="23">
-        <v>1197</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="F74" s="23"/>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-    </row>
-    <row r="76" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>183</v>
+      </c>
+      <c r="D74" s="16">
+        <v>12345</v>
+      </c>
+      <c r="E74" s="31"/>
+    </row>
+    <row r="75" spans="1:6" s="16" customFormat="1" ht="28">
+      <c r="A75" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E75" s="31"/>
+      <c r="F75" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="16" customFormat="1">
       <c r="A76" s="16" t="s">
-        <v>186</v>
+        <v>283</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>186</v>
+        <v>283</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>186</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="16" customFormat="1" ht="42">
+        <v>293</v>
+      </c>
+      <c r="E76" s="31"/>
+    </row>
+    <row r="77" spans="1:6" s="16" customFormat="1">
       <c r="A77" s="16" t="s">
-        <v>262</v>
+        <v>187</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>262</v>
+        <v>187</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D77" s="16">
-        <v>12345</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="16" customFormat="1" ht="28">
-      <c r="A78" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="B78" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="16" customFormat="1" ht="42">
+      <c r="D77" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="E77" s="31"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="19"/>
+    </row>
+    <row r="79" spans="1:6" ht="70">
       <c r="A79" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="16" customFormat="1" ht="42">
-      <c r="A80" s="16" t="s">
+      <c r="E79" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="F79" s="16" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="70">
+      <c r="A80" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C80" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>339</v>
+      <c r="D80" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-    </row>
-    <row r="82" spans="1:6" ht="42">
+      <c r="A81" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D81" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F81" s="16"/>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="16" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>307</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="F82" s="16" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="42">
-      <c r="A83" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="42">
+        <v>297</v>
+      </c>
+      <c r="F82" s="16"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F83" s="16"/>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="16" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="1:6" ht="42">
-      <c r="A85" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C85" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="F85" s="16"/>
-    </row>
-    <row r="86" spans="1:6" ht="42">
-      <c r="A86" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C86" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D86" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="F86" s="16"/>
-    </row>
-    <row r="87" spans="1:6" ht="42">
-      <c r="A87" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C87" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D87" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="F87" s="16"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="18" t="s">
+    <row r="85" spans="1:6">
+      <c r="A85" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="19"/>
+    </row>
+    <row r="86" spans="1:6" ht="41" customHeight="1">
+      <c r="A86" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E86" s="21"/>
+    </row>
+    <row r="87" spans="1:6" ht="28">
+      <c r="A87" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="28">
+      <c r="A88" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="70">
+      <c r="A89" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D89" s="24">
+        <v>42305</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="19"/>
+    </row>
+    <row r="91" spans="1:6" ht="56">
+      <c r="A91" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-    </row>
-    <row r="89" spans="1:6" ht="42">
-      <c r="A89" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="E89" s="13" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="42">
-      <c r="A90" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="F90" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28">
-      <c r="A91" s="28" t="s">
-        <v>266</v>
-      </c>
       <c r="B91" s="13" t="s">
-        <v>221</v>
+        <v>337</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>197</v>
+        <v>138</v>
+      </c>
+      <c r="D91" s="13" t="b">
+        <v>0</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated citation mapping and XML instance.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="320" windowWidth="28800" windowHeight="17940"/>
+    <workbookView xWindow="2620" yWindow="1900" windowWidth="28800" windowHeight="17940"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="291">
   <si>
     <t>Description</t>
   </si>
@@ -613,21 +613,6 @@
   </si>
   <si>
     <t>Posteds peed unit of measure</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We should also include the Xpath for residence association to indicate that a location needs to be association to a person
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I'll include the Associations in the mapping.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -642,21 +627,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Agreed.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Let's spell this out, not FAW acronym unless that is a commonly used acronym of which I am not aware
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OK</t>
     </r>
   </si>
   <si>
@@ -744,31 +714,13 @@
     <t>Citation Mailed Indicator</t>
   </si>
   <si>
-    <t>How do we know this is a citation?
-I'm not sure about your question, Vermont calls this a "Citation Number"</t>
-  </si>
-  <si>
     <t>The date the citation was served to the subject.</t>
   </si>
   <si>
-    <t>Instead of "citation" the proper term is probably "citation".  Also, can you please check the definition of this element in schema, doesn’t seem right. 
-I'll change all occurences of "Citation" to "Citation" and check definitions</t>
-  </si>
-  <si>
     <t>Indicates that the citation/citation was handed to the subject.</t>
   </si>
   <si>
     <t>Indicates that thecitation/citation was mailed to the subject.</t>
-  </si>
-  <si>
-    <t>Presumably there is an association between the citation at he organization to make it clear that the organization received the citation?
-Yes there is.  I'll include the Association in the spreadsheet</t>
-  </si>
-  <si>
-    <t>If there are multiple people in the report, how do we know which one received the citation?
-Citation (Citation) Incident Association
-Person In cident Association
-I'll include Associations in tha mapping</t>
   </si>
   <si>
     <t>LICENSE</t>
@@ -944,13 +896,6 @@
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/j:PersonDriverLicenseAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:DriverLicenseReference/@s:ref]/inc-ext:DriverLicenseCDLIndicator</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[nc:ActivityCategoryText=’true'][@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation
-[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Vehicle[ndexia:VehicleAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/@s:id]/nc:VehicleCMVIndicator</t>
   </si>
   <si>
@@ -977,6 +922,59 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location
+[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location
+[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode
+</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation
+[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:PersonBirthLocationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:LocationReference/@s:ref]</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/j:ActivityEnforcementOfficialAssociation/nc:PersonReference/@s:ref]/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Organization[ndexia:OrganizationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>NEED TO DETERMINE FROM VT HOW TO HANDLE</t>
   </si>
 </sst>
 </file>
@@ -986,7 +984,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,12 +1073,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF6600"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -1199,7 +1191,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="510">
+  <cellStyleXfs count="530">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1710,8 +1702,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1723,9 +1735,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1752,13 +1761,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1777,7 +1783,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="510">
+  <cellStyles count="530">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2041,6 +2047,16 @@
     <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2283,6 +2299,16 @@
     <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2590,35 +2616,35 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.83203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="105.83203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="42">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="42">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2630,11 +2656,11 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="17"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="4"/>
@@ -2642,51 +2668,46 @@
         <v>83</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="70">
       <c r="A4" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D4" s="2">
         <v>82734800</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>210</v>
+      <c r="E4" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A5" s="7" t="s">
-        <v>207</v>
+      <c r="A5" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>42304</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>212</v>
-      </c>
+      <c r="E5" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -2695,20 +2716,20 @@
       <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>105</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="10"/>
+      <c r="E6" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A7" s="7" t="s">
-        <v>208</v>
+      <c r="A7" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>50</v>
@@ -2716,16 +2737,16 @@
       <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>266</v>
+      <c r="E7" s="13" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A8" s="7" t="s">
-        <v>209</v>
+      <c r="A8" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>51</v>
@@ -2733,75 +2754,69 @@
       <c r="D8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>268</v>
+      <c r="E8" s="13" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="70">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>215</v>
+      <c r="E10" s="12" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="70">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>215</v>
+        <v>274</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="84">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="70">
       <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
@@ -2814,11 +2829,8 @@
       <c r="D14" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>216</v>
+      <c r="E14" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="70">
@@ -2834,8 +2846,8 @@
       <c r="D15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>229</v>
+      <c r="E15" s="12" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="70">
@@ -2851,11 +2863,11 @@
       <c r="D16" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="56">
+      <c r="E16" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="112">
       <c r="A17" s="2" t="s">
         <v>59</v>
       </c>
@@ -2868,12 +2880,11 @@
       <c r="D17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="E17" s="12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="112">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -2886,9 +2897,11 @@
       <c r="D18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="140">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -2901,8 +2914,11 @@
       <c r="D19" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1">
+      <c r="E19" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -2915,7 +2931,9 @@
       <c r="D20" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="13" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="84">
       <c r="A21" s="2" t="s">
@@ -2930,8 +2948,8 @@
       <c r="D21" s="2">
         <v>41444812</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>231</v>
+      <c r="E21" s="17" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="84">
@@ -2947,8 +2965,8 @@
       <c r="D22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>232</v>
+      <c r="E22" s="17" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="140">
@@ -2964,11 +2982,8 @@
       <c r="D23" s="2">
         <v>12345678</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>200</v>
+      <c r="E23" s="17" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="112">
@@ -2984,11 +2999,11 @@
       <c r="D24" s="3">
         <v>8023631111</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="E24" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -3001,8 +3016,8 @@
       <c r="D25" s="3">
         <v>8023631112</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>274</v>
+      <c r="E25" s="6" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3015,13 +3030,13 @@
       <c r="C26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <v>24014</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="F26" s="9"/>
+      <c r="E26" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A27" s="3" t="s">
@@ -3036,11 +3051,11 @@
       <c r="D27" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1">
+      <c r="E27" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A28" s="3" t="s">
         <v>165</v>
       </c>
@@ -3053,7 +3068,9 @@
       <c r="D28" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="6" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A29" s="3" t="s">
@@ -3068,8 +3085,8 @@
       <c r="D29" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="19" t="s">
-        <v>235</v>
+      <c r="E29" s="17" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3079,8 +3096,8 @@
       <c r="B30" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>236</v>
+      <c r="E30" s="17" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3096,8 +3113,8 @@
       <c r="D31" s="3">
         <v>135</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>237</v>
+      <c r="E31" s="17" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3107,8 +3124,8 @@
       <c r="B32" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>238</v>
+      <c r="E32" s="17" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3124,8 +3141,8 @@
       <c r="D33" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>239</v>
+      <c r="E33" s="17" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3141,19 +3158,19 @@
       <c r="D34" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>240</v>
+      <c r="E34" s="17" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="6"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A36" s="3" t="s">
@@ -3168,8 +3185,8 @@
       <c r="D36" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>221</v>
+      <c r="E36" s="13" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3182,8 +3199,8 @@
       <c r="D37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>222</v>
+      <c r="E37" s="13" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3199,8 +3216,8 @@
       <c r="D38" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>223</v>
+      <c r="E38" s="13" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3216,8 +3233,8 @@
       <c r="D39" s="3">
         <v>2015</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>220</v>
+      <c r="E39" s="13" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3233,8 +3250,8 @@
       <c r="D40" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>224</v>
+      <c r="E40" s="13" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3250,8 +3267,8 @@
       <c r="D41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>225</v>
+      <c r="E41" s="13" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3267,8 +3284,8 @@
       <c r="D42" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>226</v>
+      <c r="E42" s="13" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3284,12 +3301,12 @@
       <c r="D43" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>276</v>
+      <c r="E43" s="13" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -3301,19 +3318,19 @@
       <c r="D44" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>277</v>
+      <c r="E44" s="13" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="6"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A46" s="2" t="s">
@@ -3328,11 +3345,11 @@
       <c r="D46" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>261</v>
+      <c r="E46" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="42">
@@ -3345,26 +3362,26 @@
       <c r="C47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="F47" s="9"/>
+      <c r="E47" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" s="3" customFormat="1" ht="126">
       <c r="A48" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>278</v>
+      <c r="E48" s="13" t="s">
+        <v>270</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>162</v>
@@ -3383,8 +3400,8 @@
       <c r="D49" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>269</v>
+      <c r="E49" s="13" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3400,8 +3417,8 @@
       <c r="D50" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>270</v>
+      <c r="E50" s="13" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="42">
@@ -3417,12 +3434,12 @@
       <c r="D51" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>271</v>
+      <c r="E51" s="13" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -3434,15 +3451,15 @@
       <c r="D52" s="3">
         <v>0.2</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>245</v>
+      <c r="E52" s="13" t="s">
+        <v>239</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -3454,12 +3471,12 @@
       <c r="D53" s="3">
         <v>30</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>243</v>
+      <c r="E53" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3468,12 +3485,12 @@
       <c r="D54" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>244</v>
+      <c r="E54" s="13" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -3485,12 +3502,12 @@
       <c r="D55" s="3">
         <v>40</v>
       </c>
-      <c r="E55" s="15" t="s">
-        <v>247</v>
+      <c r="E55" s="13" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3499,12 +3516,12 @@
       <c r="D56" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E56" s="15" t="s">
-        <v>246</v>
+      <c r="E56" s="13" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3516,12 +3533,12 @@
       <c r="D57" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E57" s="15" t="s">
-        <v>248</v>
+      <c r="E57" s="13" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3533,12 +3550,12 @@
       <c r="D58" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E58" s="15" t="s">
-        <v>249</v>
+      <c r="E58" s="13" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -3550,12 +3567,12 @@
       <c r="D59" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E59" s="15" t="s">
-        <v>250</v>
+      <c r="E59" s="13" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="70">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -3567,12 +3584,12 @@
       <c r="D60" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E60" s="15" t="s">
-        <v>251</v>
+      <c r="E60" s="13" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="70">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -3584,12 +3601,12 @@
       <c r="D61" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E61" s="15" t="s">
-        <v>252</v>
+      <c r="E61" s="13" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="70">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -3601,12 +3618,12 @@
       <c r="D62" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E62" s="13" t="s">
-        <v>253</v>
+      <c r="E62" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="70">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>158</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -3615,19 +3632,19 @@
       <c r="D63" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E63" s="13" t="s">
-        <v>254</v>
+      <c r="E63" s="12" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="6"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A65" s="3" t="s">
@@ -3642,12 +3659,12 @@
       <c r="D65" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>263</v>
+      <c r="E65" s="13" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -3659,12 +3676,12 @@
       <c r="D66" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>256</v>
+      <c r="E66" s="13" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -3676,12 +3693,12 @@
       <c r="D67" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E67" s="15" t="s">
-        <v>255</v>
+      <c r="E67" s="13" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -3693,12 +3710,12 @@
       <c r="D68" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>257</v>
+      <c r="E68" s="13" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -3710,13 +3727,13 @@
       <c r="D69" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E69" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="F69" s="7"/>
+      <c r="E69" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -3728,12 +3745,12 @@
       <c r="D70" s="3">
         <v>2</v>
       </c>
-      <c r="E70" s="15" t="s">
-        <v>258</v>
+      <c r="E70" s="13" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="6" t="s">
         <v>122</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -3742,16 +3759,16 @@
       <c r="C71" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="9">
         <v>47</v>
       </c>
-      <c r="E71" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="F71" s="10"/>
+      <c r="E71" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -3760,23 +3777,23 @@
       <c r="C72" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="9">
         <v>1197</v>
       </c>
-      <c r="E72" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="F72" s="10"/>
+      <c r="E72" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="6"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A74" s="3" t="s">
@@ -3791,11 +3808,11 @@
       <c r="D74" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E74" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1">
+      <c r="E74" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A75" s="3" t="s">
         <v>117</v>
       </c>
@@ -3808,24 +3825,28 @@
       <c r="D75" s="3">
         <v>12345</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="76" spans="1:6" s="3" customFormat="1" ht="28">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E76" s="15"/>
+      <c r="E76" s="6" t="s">
+        <v>290</v>
+      </c>
       <c r="F76" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="3" customFormat="1">
+    <row r="77" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A77" s="3" t="s">
         <v>143</v>
       </c>
@@ -3838,9 +3859,11 @@
       <c r="D77" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="1:6" s="3" customFormat="1">
+      <c r="E77" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -3853,17 +3876,19 @@
       <c r="D78" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="13" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="6"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" ht="70">
       <c r="A80" s="3" t="s">
@@ -3878,11 +3903,11 @@
       <c r="D80" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E80" s="13" t="s">
-        <v>219</v>
+      <c r="E80" s="12" t="s">
+        <v>213</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="70">
@@ -3898,11 +3923,11 @@
       <c r="D81" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E81" s="13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="E81" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="112">
       <c r="A82" s="3" t="s">
         <v>59</v>
       </c>
@@ -3915,9 +3940,12 @@
       <c r="D82" s="3" t="s">
         <v>155</v>
       </c>
+      <c r="E82" s="12" t="s">
+        <v>280</v>
+      </c>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" ht="112">
       <c r="A83" s="3" t="s">
         <v>4</v>
       </c>
@@ -3930,9 +3958,12 @@
       <c r="D83" s="3" t="s">
         <v>156</v>
       </c>
+      <c r="E83" s="12" t="s">
+        <v>281</v>
+      </c>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" ht="126">
       <c r="A84" s="3" t="s">
         <v>5</v>
       </c>
@@ -3945,9 +3976,12 @@
       <c r="D84" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="E84" s="12" t="s">
+        <v>283</v>
+      </c>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" ht="112">
       <c r="A85" s="3" t="s">
         <v>6</v>
       </c>
@@ -3960,20 +3994,23 @@
       <c r="D85" s="3" t="s">
         <v>157</v>
       </c>
+      <c r="E85" s="12" t="s">
+        <v>282</v>
+      </c>
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="6"/>
+      <c r="A86" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" ht="98">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -3985,16 +4022,16 @@
       <c r="D87" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E87" s="13" t="s">
-        <v>273</v>
+      <c r="E87" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="119" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating mappings for driver license, home phone and business phone
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="1900" windowWidth="28800" windowHeight="17940"/>
+    <workbookView xWindow="2420" yWindow="500" windowWidth="31480" windowHeight="17940"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="286">
   <si>
     <t>Description</t>
   </si>
@@ -501,15 +501,9 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>We need a decision on whether to include this element and if so what format.</t>
-  </si>
-  <si>
     <t>Commerical Vehicle Indicator</t>
   </si>
   <si>
-    <t>This element appears to be a duplicate of the Officer Agency ORI.  We need to know what this element should be.</t>
-  </si>
-  <si>
     <t>Hair Color Code</t>
   </si>
   <si>
@@ -613,86 +607,6 @@
   </si>
   <si>
     <t>Posteds peed unit of measure</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Wouldn’t this be better modeled as a property of a driver license, not a person?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Agreed.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Shouldn’t this be: /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[nc:ActivityCategoryText='Incident']</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/nc:ActivityIdentification/nc:IdentificationID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OK</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">there isn't a concept for this in NIEM or N-Dex?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NIEM only has "ArrestBloodAlcoholContentNumberText"
-ECF has "PersonBloodAlcoholNumber"… I can use this.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We should indicate the Association Xpath in here
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I'll add Associations to the spreadsheet</t>
-    </r>
   </si>
   <si>
     <t>eCitation Element
@@ -893,9 +807,6 @@
 </t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/j:PersonDriverLicenseAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:DriverLicenseReference/@s:ref]/inc-ext:DriverLicenseCDLIndicator</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Vehicle[ndexia:VehicleAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/@s:id]/nc:VehicleCMVIndicator</t>
   </si>
   <si>
@@ -958,23 +869,30 @@
 </t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/j:ActivityEnforcementOfficialAssociation/nc:PersonReference/@s:ref]/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Organization[ndexia:OrganizationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberWorkIndicator='true']
 [nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:PersonBirthLocationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:LocationReference/@s:ref]</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/j:ActivityEnforcementOfficialAssociation/nc:PersonReference/@s:ref]/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Organization[ndexia:OrganizationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>NEED TO DETERMINE FROM VT HOW TO HANDLE</t>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberHomeIndicator='true']
+[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>not required</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref= /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id = ../j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/@s:id]/inc-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -2615,8 +2533,8 @@
   <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2633,13 +2551,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="42">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>124</v>
@@ -2673,27 +2591,27 @@
     </row>
     <row r="4" spans="1:6" ht="70">
       <c r="A4" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D4" s="2">
         <v>82734800</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>49</v>
@@ -2702,7 +2620,7 @@
         <v>42304</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -2711,7 +2629,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>48</v>
@@ -2720,16 +2638,16 @@
         <v>105</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>50</v>
@@ -2738,15 +2656,15 @@
         <v>1</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A8" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>51</v>
@@ -2755,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2773,18 +2691,18 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2797,13 +2715,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2830,7 +2748,7 @@
         <v>127</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="70">
@@ -2847,7 +2765,7 @@
         <v>128</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="70">
@@ -2864,7 +2782,7 @@
         <v>129</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="112">
@@ -2881,7 +2799,7 @@
         <v>130</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="112">
@@ -2898,7 +2816,7 @@
         <v>131</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="140">
@@ -2915,7 +2833,7 @@
         <v>125</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" ht="112">
@@ -2932,7 +2850,7 @@
         <v>132</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="84">
@@ -2949,7 +2867,7 @@
         <v>41444812</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="84">
@@ -2957,7 +2875,7 @@
         <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -2966,7 +2884,7 @@
         <v>125</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="140">
@@ -2983,7 +2901,7 @@
         <v>12345678</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="112">
@@ -2991,7 +2909,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
@@ -2999,8 +2917,8 @@
       <c r="D24" s="3">
         <v>8023631111</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>285</v>
+      <c r="E24" s="13" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3008,7 +2926,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>17</v>
@@ -3016,8 +2934,8 @@
       <c r="D25" s="3">
         <v>8023631112</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>285</v>
+      <c r="E25" s="13" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3034,7 +2952,7 @@
         <v>24014</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -3052,15 +2970,15 @@
         <v>133</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="98">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>19</v>
@@ -3069,7 +2987,7 @@
         <v>134</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3086,18 +3004,18 @@
         <v>135</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A30" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3114,7 +3032,7 @@
         <v>135</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3122,18 +3040,18 @@
         <v>121</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A33" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
@@ -3142,15 +3060,15 @@
         <v>136</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A34" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>23</v>
@@ -3159,7 +3077,7 @@
         <v>136</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3183,10 +3101,10 @@
         <v>68</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3200,7 +3118,7 @@
         <v>137</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3208,7 +3126,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -3217,7 +3135,7 @@
         <v>125</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3225,7 +3143,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>24</v>
@@ -3234,7 +3152,7 @@
         <v>2015</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3242,7 +3160,7 @@
         <v>100</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>25</v>
@@ -3251,7 +3169,7 @@
         <v>139</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3259,7 +3177,7 @@
         <v>101</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>26</v>
@@ -3268,7 +3186,7 @@
         <v>140</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3276,7 +3194,7 @@
         <v>102</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>27</v>
@@ -3285,15 +3203,15 @@
         <v>141</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A43" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>39</v>
@@ -3302,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3319,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3332,12 +3250,12 @@
       <c r="E45" s="16"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="98">
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>104</v>
@@ -3346,11 +3264,9 @@
         <v>126</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>199</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A47" s="3" t="s">
@@ -3366,7 +3282,7 @@
         <v>142</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -3375,16 +3291,13 @@
         <v>106</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>162</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3392,7 +3305,7 @@
         <v>107</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>30</v>
@@ -3401,7 +3314,7 @@
         <v>144</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3418,7 +3331,7 @@
         <v>145</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="42">
@@ -3426,7 +3339,7 @@
         <v>109</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>32</v>
@@ -3435,7 +3348,7 @@
         <v>146</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3443,7 +3356,7 @@
         <v>110</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>33</v>
@@ -3452,10 +3365,7 @@
         <v>0.2</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3472,21 +3382,21 @@
         <v>30</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A54" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3503,21 +3413,21 @@
         <v>40</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A56" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3534,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3551,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3568,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="70">
@@ -3585,7 +3495,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="70">
@@ -3602,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="70">
@@ -3619,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="70">
@@ -3627,13 +3537,13 @@
         <v>158</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3648,10 +3558,10 @@
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A65" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>42</v>
@@ -3660,7 +3570,7 @@
         <v>148</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="84">
@@ -3677,12 +3587,12 @@
         <v>147</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A67" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>78</v>
@@ -3694,7 +3604,7 @@
         <v>149</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3711,15 +3621,15 @@
         <v>150</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A69" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>57</v>
@@ -3728,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F69" s="6"/>
     </row>
@@ -3746,7 +3656,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3763,7 +3673,7 @@
         <v>47</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F71" s="9"/>
     </row>
@@ -3781,7 +3691,7 @@
         <v>1197</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F72" s="9"/>
     </row>
@@ -3809,7 +3719,7 @@
         <v>151</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="3" customFormat="1" ht="84">
@@ -3826,10 +3736,10 @@
         <v>12345</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" ht="28">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1">
       <c r="A76" s="10" t="s">
         <v>54</v>
       </c>
@@ -3840,11 +3750,9 @@
         <v>54</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>160</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A77" s="3" t="s">
@@ -3860,7 +3768,7 @@
         <v>152</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3877,7 +3785,7 @@
         <v>153</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3904,11 +3812,9 @@
         <v>154</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6" ht="70">
       <c r="A81" s="2" t="s">
@@ -3924,7 +3830,7 @@
         <v>127</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="112">
@@ -3941,7 +3847,7 @@
         <v>155</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F82" s="3"/>
     </row>
@@ -3959,7 +3865,7 @@
         <v>156</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F83" s="3"/>
     </row>
@@ -3977,7 +3883,7 @@
         <v>125</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="F84" s="3"/>
     </row>
@@ -3995,13 +3901,13 @@
         <v>157</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="18" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -4009,12 +3915,12 @@
       <c r="E86" s="16"/>
       <c r="F86" s="5"/>
     </row>
-    <row r="87" spans="1:6" ht="98">
+    <row r="87" spans="1:6" ht="84">
       <c r="A87" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>8</v>
@@ -4023,15 +3929,12 @@
         <v>0</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="119" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>